<commit_message>
I don't remembre where i was
</commit_message>
<xml_diff>
--- a/app/code/data/excels/copy_expenses.xlsx
+++ b/app/code/data/excels/copy_expenses.xlsx
@@ -15,10 +15,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1614502180" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1614502180" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1614502180" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1614502180"/>
+      <pm:revision xmlns:pm="smNativeData" day="1616078867" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1616078867" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1616078867" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1616078867"/>
     </ext>
   </extLst>
 </workbook>
@@ -1273,7 +1273,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614502180" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1616078867" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1288,7 +1288,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614502180" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1616078867" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1304,7 +1304,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614502180" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1616078867" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -1319,7 +1319,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1614502180" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1616078867" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="240" lang="default"/>
             <pm:ea face="Basic Roman" sz="240" lang="default"/>
@@ -1328,7 +1328,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1359,8 +1359,19 @@
     <fill>
       <patternFill patternType="none"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1616078867" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -1376,7 +1387,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614502180"/>
+          <pm:border xmlns:pm="smNativeData" id="1616078867"/>
         </ext>
       </extLst>
     </border>
@@ -1395,7 +1406,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614502180">
+          <pm:border xmlns:pm="smNativeData" id="1616078867">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1416,7 +1427,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614502180">
+          <pm:border xmlns:pm="smNativeData" id="1616078867">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1438,7 +1449,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614502180">
+          <pm:border xmlns:pm="smNativeData" id="1616078867">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1459,7 +1470,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614502180">
+          <pm:border xmlns:pm="smNativeData" id="1616078867">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1480,7 +1491,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614502180">
+          <pm:border xmlns:pm="smNativeData" id="1616078867">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1502,7 +1513,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614502180">
+          <pm:border xmlns:pm="smNativeData" id="1616078867">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -1525,7 +1536,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614502180">
+          <pm:border xmlns:pm="smNativeData" id="1616078867">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1547,9 +1558,28 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1614502180">
+          <pm:border xmlns:pm="smNativeData" id="1616078867">
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1616078867"/>
         </ext>
       </extLst>
     </border>
@@ -1628,10 +1658,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1614502180" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1616078867" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1614502180" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1616078867" count="1">
         <pm:color name="Gris 20%" rgb="000000"/>
       </pm:colors>
     </ext>
@@ -1897,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K624"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G11"/>
+    <sheetView tabSelected="1" view="normal" zoomScale="150" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.553571" defaultRowHeight="15.40"/>
@@ -2118,7 +2148,7 @@
       </c>
       <c r="B12" s="4"/>
       <c r="C12" t="n">
-        <v>10.3399999999999999</v>
+        <v>10.3400000000000016</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>25</v>
@@ -3263,7 +3293,7 @@
       </c>
       <c r="B93" s="4"/>
       <c r="C93" t="n">
-        <v>13.9199999999999999</v>
+        <v>13.9200000000000017</v>
       </c>
       <c r="D93" s="12" t="s">
         <v>103</v>
@@ -3547,7 +3577,7 @@
       </c>
       <c r="B114" s="2"/>
       <c r="C114" s="3" t="n">
-        <v>10.3399999999999999</v>
+        <v>10.3400000000000016</v>
       </c>
       <c r="D114" s="13" t="s">
         <v>120</v>
@@ -5637,7 +5667,7 @@
       </c>
       <c r="B267" s="2"/>
       <c r="C267" s="3" t="n">
-        <v>11.4199999999999999</v>
+        <v>11.4200000000000017</v>
       </c>
       <c r="D267" s="13" t="s">
         <v>232</v>
@@ -7846,7 +7876,7 @@
       </c>
       <c r="B432" s="2"/>
       <c r="C432" s="3" t="n">
-        <v>114.109999999999999</v>
+        <v>114.110000000000014</v>
       </c>
       <c r="D432" s="13" t="s">
         <v>92</v>
@@ -9886,7 +9916,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1614502180" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1616078867" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -9895,14 +9925,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1614502180" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1614502180" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1616078867" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1616078867" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614502180" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1616078867" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -9924,7 +9954,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1614502180" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1616078867" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -9933,14 +9963,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1614502180" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1614502180" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1616078867" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1616078867" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614502180" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1616078867" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -9962,7 +9992,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1614502180" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1616078867" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -9971,14 +10001,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1614502180" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1614502180" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1616078867" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1616078867" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1614502180" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1616078867" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>